<commit_message>
cols wrong in template
</commit_message>
<xml_diff>
--- a/testsheets/666_Tektronix_DPO20141.xlsx
+++ b/testsheets/666_Tektronix_DPO20141.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Software\Python\oscilloscope\testsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{21F56171-0DF3-4EE6-BA5E-BF9D3C4C3FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F620F81-795C-4C7C-8294-08F8271C05F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1598,7 +1598,7 @@
   </sheetPr>
   <dimension ref="A1:S104"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A5" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2712,12 +2712,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>25</v>
       </c>
@@ -2736,15 +2736,15 @@
       <c r="F66" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="M66" s="10" t="s">
+      <c r="N66" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="N66" s="10"/>
-      <c r="O66" s="10" t="s">
+      <c r="O66" s="10"/>
+      <c r="P66" s="10" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>52</v>
       </c>
@@ -2763,17 +2763,17 @@
         <f>IF(ISBLANK(B67),"Not Done",IF(D67&gt;=C67,"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="M67" s="10" t="s">
+      <c r="N67" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="N67" s="10">
+      <c r="O67" s="10">
         <v>1</v>
       </c>
-      <c r="O67" s="10">
+      <c r="P67" s="10">
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>54</v>
       </c>
@@ -2792,17 +2792,17 @@
         <f>IF(ISBLANK(B68),"Not Done",IF(D68&gt;=C68,"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="M68" s="10" t="s">
+      <c r="N68" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="N68" s="10">
+      <c r="O68" s="10">
         <v>2</v>
       </c>
-      <c r="O68" s="10">
+      <c r="P68" s="10">
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
         <v>55</v>
       </c>
@@ -2821,17 +2821,17 @@
         <f>IF(ISBLANK(B69),"Not Done",IF(D69&gt;=C69,"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="M69" s="10" t="s">
+      <c r="N69" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="N69" s="10">
+      <c r="O69" s="10">
         <v>3</v>
       </c>
-      <c r="O69" s="10">
+      <c r="P69" s="10">
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>56</v>
       </c>
@@ -2850,22 +2850,22 @@
         <f>IF(ISBLANK(B70),"Not Done",IF(D70&gt;=C70,"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="M70" s="10" t="s">
+      <c r="N70" s="10" t="s">
         <v>79</v>
-      </c>
-      <c r="N70" s="10">
-        <v>4</v>
       </c>
       <c r="O70" s="10">
         <v>4</v>
       </c>
-    </row>
-    <row r="72" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P70" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>25</v>
       </c>
@@ -2876,7 +2876,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
         <v>58</v>
       </c>
@@ -2888,7 +2888,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
         <v>59</v>
       </c>
@@ -2900,7 +2900,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
         <v>60</v>
       </c>
@@ -2912,7 +2912,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
         <v>61</v>
       </c>
@@ -2924,12 +2924,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>25</v>
       </c>
@@ -3092,7 +3092,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
         <v>60</v>
       </c>
@@ -3104,7 +3104,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
         <v>61</v>
       </c>
@@ -3116,12 +3116,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="100" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>25</v>
       </c>
@@ -3140,11 +3140,11 @@
       <c r="F101" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="M101" s="10" t="s">
+      <c r="N101" s="10" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
         <v>65</v>
       </c>
@@ -3162,14 +3162,14 @@
         <f>IF(ISBLANK(C102),"Not Done",IF(AND(C102&lt;=D102,C102&gt;=B102),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="M102" s="10" t="s">
+      <c r="N102" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="O102" s="10">
+      <c r="P102" s="10">
         <v>10</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C104" s="9" t="s">
         <v>67</v>
       </c>

</xml_diff>

<commit_message>
update template for dcv test
</commit_message>
<xml_diff>
--- a/testsheets/666_Tektronix_DPO20141.xlsx
+++ b/testsheets/666_Tektronix_DPO20141.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Software\Python\oscilloscope\testsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F620F81-795C-4C7C-8294-08F8271C05F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC0A5C17-8DB1-423B-A9C6-420D292D86D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="80">
   <si>
     <t>EMU Filename:</t>
   </si>
@@ -257,9 +257,6 @@
   </si>
   <si>
     <t>Scale</t>
-  </si>
-  <si>
-    <t>y</t>
   </si>
   <si>
     <t>BAL</t>
@@ -362,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -389,6 +386,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1596,7 +1600,7 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S104"/>
+  <dimension ref="A1:T104"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -1608,6 +1612,7 @@
     <col min="2" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
     <col min="6" max="7" width="16" customWidth="1"/>
+    <col min="14" max="20" width="9.140625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -1739,12 +1744,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>25</v>
       </c>
@@ -1755,7 +1760,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>29</v>
       </c>
@@ -1767,33 +1772,33 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="M21" s="10" t="s">
+      <c r="N21" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="N21" s="10" t="s">
+      <c r="O21" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="O21" s="10" t="s">
+      <c r="P21" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="P21" s="10" t="s">
+      <c r="Q21" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="Q21" s="10" t="s">
+      <c r="R21" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="R21" s="10" t="s">
+      <c r="S21" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="T21" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="S21" s="10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>25</v>
       </c>
@@ -1814,7 +1819,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>35</v>
       </c>
@@ -1822,7 +1827,7 @@
       <c r="C23" s="6">
         <v>-21</v>
       </c>
-      <c r="D23" s="6"/>
+      <c r="D23" s="12"/>
       <c r="E23" s="6">
         <v>21</v>
       </c>
@@ -1833,23 +1838,23 @@
         <f>IF(ISBLANK(D23),"Not Done",IF(AND(D23&lt;=E23,D23&gt;=C23),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="N23" t="s">
-        <v>74</v>
-      </c>
-      <c r="O23">
+      <c r="N23" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="O23" s="10">
         <v>1</v>
       </c>
-      <c r="P23" t="s">
+      <c r="P23" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="Q23">
+      <c r="Q23" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="R23">
+      <c r="R23" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>37</v>
       </c>
@@ -1857,7 +1862,7 @@
       <c r="C24" s="6">
         <v>-21</v>
       </c>
-      <c r="D24" s="6"/>
+      <c r="D24" s="12"/>
       <c r="E24" s="6">
         <v>21</v>
       </c>
@@ -1868,29 +1873,33 @@
         <f>IF(ISBLANK(D24),"Not Done",IF(AND(D24&lt;=E24,D24&gt;=C24),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="N24" t="s">
-        <v>74</v>
-      </c>
-      <c r="O24">
+      <c r="N24" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="O24" s="10">
         <v>1</v>
       </c>
-      <c r="P24" t="s">
+      <c r="P24" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="Q24">
+      <c r="Q24" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="R24">
+      <c r="R24" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="D25" s="13"/>
+    </row>
+    <row r="26" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B26" s="4"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D26" s="13"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>25</v>
       </c>
@@ -1898,7 +1907,7 @@
       <c r="C27" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="14" t="s">
         <v>32</v>
       </c>
       <c r="E27" s="5" t="s">
@@ -1911,7 +1920,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>35</v>
       </c>
@@ -1919,7 +1928,7 @@
       <c r="C28" s="6">
         <v>-21</v>
       </c>
-      <c r="D28" s="6"/>
+      <c r="D28" s="12"/>
       <c r="E28" s="6">
         <v>21</v>
       </c>
@@ -1930,23 +1939,23 @@
         <f>IF(ISBLANK(D28),"Not Done",IF(AND(D28&lt;=E28,D28&gt;=C28),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="N28" t="s">
-        <v>74</v>
-      </c>
-      <c r="O28">
+      <c r="N28" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="O28" s="10">
         <v>2</v>
       </c>
-      <c r="P28" t="s">
+      <c r="P28" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="Q28">
+      <c r="Q28" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="R28">
+      <c r="R28" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>37</v>
       </c>
@@ -1954,7 +1963,7 @@
       <c r="C29" s="6">
         <v>-21</v>
       </c>
-      <c r="D29" s="6"/>
+      <c r="D29" s="12"/>
       <c r="E29" s="6">
         <v>21</v>
       </c>
@@ -1965,29 +1974,33 @@
         <f>IF(ISBLANK(D29),"Not Done",IF(AND(D29&lt;=E29,D29&gt;=C29),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="N29" t="s">
-        <v>74</v>
-      </c>
-      <c r="O29">
+      <c r="N29" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="O29" s="10">
         <v>2</v>
       </c>
-      <c r="P29" t="s">
+      <c r="P29" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="Q29">
+      <c r="Q29" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="R29">
+      <c r="R29" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="D30" s="13"/>
+    </row>
+    <row r="31" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B31" s="4"/>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D31" s="13"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>25</v>
       </c>
@@ -1995,7 +2008,7 @@
       <c r="C32" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="14" t="s">
         <v>32</v>
       </c>
       <c r="E32" s="5" t="s">
@@ -2008,7 +2021,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>35</v>
       </c>
@@ -2016,7 +2029,7 @@
       <c r="C33" s="6">
         <v>-21</v>
       </c>
-      <c r="D33" s="6"/>
+      <c r="D33" s="12"/>
       <c r="E33" s="6">
         <v>21</v>
       </c>
@@ -2027,23 +2040,23 @@
         <f>IF(ISBLANK(D33),"Not Done",IF(AND(D33&lt;=E33,D33&gt;=C33),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="N33" t="s">
-        <v>74</v>
-      </c>
-      <c r="O33">
+      <c r="N33" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="O33" s="10">
         <v>3</v>
       </c>
-      <c r="P33" t="s">
+      <c r="P33" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="Q33">
+      <c r="Q33" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="R33">
+      <c r="R33" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>37</v>
       </c>
@@ -2051,7 +2064,7 @@
       <c r="C34" s="6">
         <v>-21</v>
       </c>
-      <c r="D34" s="6"/>
+      <c r="D34" s="12"/>
       <c r="E34" s="6">
         <v>21</v>
       </c>
@@ -2062,29 +2075,33 @@
         <f>IF(ISBLANK(D34),"Not Done",IF(AND(D34&lt;=E34,D34&gt;=C34),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="N34" t="s">
-        <v>74</v>
-      </c>
-      <c r="O34">
+      <c r="N34" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="O34" s="10">
         <v>3</v>
       </c>
-      <c r="P34" t="s">
+      <c r="P34" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="Q34">
+      <c r="Q34" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="R34">
+      <c r="R34" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D35" s="13"/>
+    </row>
+    <row r="36" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B36" s="4"/>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D36" s="13"/>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>25</v>
       </c>
@@ -2092,7 +2109,7 @@
       <c r="C37" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="14" t="s">
         <v>32</v>
       </c>
       <c r="E37" s="5" t="s">
@@ -2105,7 +2122,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>35</v>
       </c>
@@ -2113,7 +2130,7 @@
       <c r="C38" s="6">
         <v>-21</v>
       </c>
-      <c r="D38" s="6"/>
+      <c r="D38" s="12"/>
       <c r="E38" s="6">
         <v>21</v>
       </c>
@@ -2124,23 +2141,23 @@
         <f>IF(ISBLANK(D38),"Not Done",IF(AND(D38&lt;=E38,D38&gt;=C38),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="N38" t="s">
-        <v>74</v>
-      </c>
-      <c r="O38">
+      <c r="N38" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="O38" s="10">
         <v>4</v>
       </c>
-      <c r="P38" t="s">
+      <c r="P38" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="Q38">
+      <c r="Q38" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="R38">
+      <c r="R38" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>37</v>
       </c>
@@ -2148,7 +2165,7 @@
       <c r="C39" s="6">
         <v>-21</v>
       </c>
-      <c r="D39" s="6"/>
+      <c r="D39" s="12"/>
       <c r="E39" s="6">
         <v>21</v>
       </c>
@@ -2159,29 +2176,29 @@
         <f>IF(ISBLANK(D39),"Not Done",IF(AND(D39&lt;=E39,D39&gt;=C39),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="N39" t="s">
-        <v>74</v>
-      </c>
-      <c r="O39">
+      <c r="N39" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="O39" s="10">
         <v>4</v>
       </c>
-      <c r="P39" t="s">
+      <c r="P39" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="Q39">
+      <c r="Q39" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="R39">
+      <c r="R39" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B41" s="4"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>25</v>
       </c>
@@ -2202,7 +2219,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>42</v>
       </c>
@@ -2221,23 +2238,26 @@
         <f>IF(ISBLANK(D43),"Not Done",IF(AND(D43&lt;=E43,D43&gt;=C43),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="N43" t="s">
-        <v>77</v>
-      </c>
-      <c r="O43">
+      <c r="N43" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="O43" s="10">
         <v>1</v>
       </c>
-      <c r="P43" t="s">
+      <c r="P43" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="Q43">
+      <c r="Q43" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="R43">
-        <v>3.5000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R43" s="10">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="S43" s="10">
+        <v>1.7500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>43</v>
       </c>
@@ -2256,23 +2276,26 @@
         <f>IF(ISBLANK(D44),"Not Done",IF(AND(D44&lt;=E44,D44&gt;=C44),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="N44" t="s">
-        <v>77</v>
-      </c>
-      <c r="O44">
+      <c r="N44" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="O44" s="10">
         <v>1</v>
       </c>
-      <c r="P44" t="s">
+      <c r="P44" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="Q44">
+      <c r="Q44" s="10">
         <v>0.2</v>
       </c>
-      <c r="R44">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R44" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="S44" s="10">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>45</v>
       </c>
@@ -2291,29 +2314,32 @@
         <f>IF(ISBLANK(D45),"Not Done",IF(AND(D45&lt;=E45,D45&gt;=C45),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="N45" t="s">
-        <v>77</v>
-      </c>
-      <c r="O45">
+      <c r="N45" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="O45" s="10">
         <v>1</v>
       </c>
-      <c r="P45" t="s">
+      <c r="P45" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="Q45">
+      <c r="Q45" s="10">
         <v>2</v>
       </c>
-      <c r="R45">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R45" s="10">
+        <v>7</v>
+      </c>
+      <c r="S45" s="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>46</v>
       </c>
       <c r="B47" s="4"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>25</v>
       </c>
@@ -2353,20 +2379,23 @@
         <f>IF(ISBLANK(D49),"Not Done",IF(AND(D49&lt;=E49,D49&gt;=C49),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="N49" t="s">
-        <v>77</v>
-      </c>
-      <c r="O49">
+      <c r="N49" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="O49" s="10">
         <v>2</v>
       </c>
-      <c r="P49" t="s">
+      <c r="P49" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="Q49">
+      <c r="Q49" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="R49">
-        <v>3.5000000000000003E-2</v>
+      <c r="R49" s="10">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="S49" s="10">
+        <v>1.7500000000000002E-2</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
@@ -2388,20 +2417,23 @@
         <f>IF(ISBLANK(D50),"Not Done",IF(AND(D50&lt;=E50,D50&gt;=C50),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="N50" t="s">
-        <v>77</v>
-      </c>
-      <c r="O50">
+      <c r="N50" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="O50" s="10">
         <v>2</v>
       </c>
-      <c r="P50" t="s">
+      <c r="P50" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="Q50">
+      <c r="Q50" s="10">
         <v>0.2</v>
       </c>
-      <c r="R50">
-        <v>1.4</v>
+      <c r="R50" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="S50" s="10">
+        <v>0.7</v>
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
@@ -2423,20 +2455,23 @@
         <f>IF(ISBLANK(D51),"Not Done",IF(AND(D51&lt;=E51,D51&gt;=C51),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="N51" t="s">
-        <v>77</v>
-      </c>
-      <c r="O51">
+      <c r="N51" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="O51" s="10">
         <v>2</v>
       </c>
-      <c r="P51" t="s">
+      <c r="P51" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="Q51">
+      <c r="Q51" s="10">
         <v>2</v>
       </c>
-      <c r="R51">
-        <v>14</v>
+      <c r="R51" s="10">
+        <v>7</v>
+      </c>
+      <c r="S51" s="10">
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
@@ -2485,20 +2520,23 @@
         <f>IF(ISBLANK(D55),"Not Done",IF(AND(D55&lt;=E55,D55&gt;=C55),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="N55" t="s">
-        <v>77</v>
-      </c>
-      <c r="O55">
+      <c r="N55" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="O55" s="10">
         <v>3</v>
       </c>
-      <c r="P55" t="s">
+      <c r="P55" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="Q55">
+      <c r="Q55" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="R55">
-        <v>3.5000000000000003E-2</v>
+      <c r="R55" s="10">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="S55" s="10">
+        <v>1.7500000000000002E-2</v>
       </c>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
@@ -2520,20 +2558,23 @@
         <f>IF(ISBLANK(D56),"Not Done",IF(AND(D56&lt;=E56,D56&gt;=C56),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="N56" t="s">
-        <v>77</v>
-      </c>
-      <c r="O56">
+      <c r="N56" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="O56" s="10">
         <v>3</v>
       </c>
-      <c r="P56" t="s">
+      <c r="P56" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="Q56">
+      <c r="Q56" s="10">
         <v>0.2</v>
       </c>
-      <c r="R56">
-        <v>1.4</v>
+      <c r="R56" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="S56" s="10">
+        <v>0.7</v>
       </c>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
@@ -2555,20 +2596,23 @@
         <f>IF(ISBLANK(D57),"Not Done",IF(AND(D57&lt;=E57,D57&gt;=C57),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="N57" t="s">
-        <v>77</v>
-      </c>
-      <c r="O57">
+      <c r="N57" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="O57" s="10">
         <v>3</v>
       </c>
-      <c r="P57" t="s">
+      <c r="P57" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="Q57">
+      <c r="Q57" s="10">
         <v>2</v>
       </c>
-      <c r="R57">
-        <v>14</v>
+      <c r="R57" s="10">
+        <v>7</v>
+      </c>
+      <c r="S57" s="10">
+        <v>7</v>
       </c>
     </row>
     <row r="59" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
@@ -2617,23 +2661,23 @@
         <f>IF(ISBLANK(D61),"Not Done",IF(AND(D61&lt;=E61,D61&gt;=C61),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="N61" t="s">
-        <v>77</v>
-      </c>
-      <c r="O61">
+      <c r="N61" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="O61" s="10">
         <v>4</v>
       </c>
-      <c r="P61" t="s">
+      <c r="P61" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="Q61">
+      <c r="Q61" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="R61">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="S61" t="s">
-        <v>73</v>
+      <c r="R61" s="10">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="S61" s="10">
+        <v>1.7500000000000002E-2</v>
       </c>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
@@ -2655,23 +2699,23 @@
         <f>IF(ISBLANK(D62),"Not Done",IF(AND(D62&lt;=E62,D62&gt;=C62),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="N62" t="s">
-        <v>77</v>
-      </c>
-      <c r="O62">
+      <c r="N62" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="O62" s="10">
         <v>4</v>
       </c>
-      <c r="P62" t="s">
+      <c r="P62" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="Q62">
+      <c r="Q62" s="10">
         <v>0.2</v>
       </c>
-      <c r="R62">
-        <v>1.4</v>
-      </c>
-      <c r="S62" t="s">
-        <v>73</v>
+      <c r="R62" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="S62" s="10">
+        <v>0.7</v>
       </c>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
@@ -2693,23 +2737,23 @@
         <f>IF(ISBLANK(D63),"Not Done",IF(AND(D63&lt;=E63,D63&gt;=C63),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="N63" t="s">
-        <v>77</v>
-      </c>
-      <c r="O63">
+      <c r="N63" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="O63" s="10">
         <v>4</v>
       </c>
-      <c r="P63" t="s">
+      <c r="P63" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="Q63">
+      <c r="Q63" s="10">
         <v>2</v>
       </c>
-      <c r="R63">
-        <v>14</v>
-      </c>
-      <c r="S63" t="s">
-        <v>73</v>
+      <c r="R63" s="10">
+        <v>7</v>
+      </c>
+      <c r="S63" s="10">
+        <v>7</v>
       </c>
     </row>
     <row r="65" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -2739,9 +2783,8 @@
       <c r="N66" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="O66" s="10"/>
       <c r="P66" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
@@ -2764,7 +2807,7 @@
         <v>Not Done</v>
       </c>
       <c r="N67" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O67" s="10">
         <v>1</v>
@@ -2793,7 +2836,7 @@
         <v>Not Done</v>
       </c>
       <c r="N68" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O68" s="10">
         <v>2</v>
@@ -2822,7 +2865,7 @@
         <v>Not Done</v>
       </c>
       <c r="N69" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O69" s="10">
         <v>3</v>
@@ -2851,7 +2894,7 @@
         <v>Not Done</v>
       </c>
       <c r="N70" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O70" s="10">
         <v>4</v>
@@ -3163,7 +3206,7 @@
         <v>Not Done</v>
       </c>
       <c r="N102" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P102" s="10">
         <v>10</v>

</xml_diff>

<commit_message>
update template for pass fail vertical pos
</commit_message>
<xml_diff>
--- a/testsheets/666_Tektronix_DPO20141.xlsx
+++ b/testsheets/666_Tektronix_DPO20141.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Software\Python\oscilloscope\testsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{189C9CE2-4E95-46D2-AFB2-3F447E98BC0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5ED815F5-DE25-43E3-B215-EEC77AF2A416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="82">
   <si>
     <t>EMU Filename:</t>
   </si>
@@ -281,6 +281,9 @@
   </si>
   <si>
     <t>POS</t>
+  </si>
+  <si>
+    <t>Result</t>
   </si>
 </sst>
 </file>
@@ -402,7 +405,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="153">
+  <dxfs count="117">
     <dxf>
       <font>
         <color rgb="FF00B050"/>
@@ -438,13 +441,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF00B050"/>
       </font>
@@ -462,13 +458,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF00B050"/>
       </font>
@@ -486,13 +475,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF00B050"/>
       </font>
@@ -510,13 +492,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF00B050"/>
       </font>
@@ -541,6 +516,104 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE699"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE699"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE699"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE699"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE699"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE699"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE699"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE699"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE699"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE699"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE699"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE699"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE699"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE699"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF00B050"/>
       </font>
@@ -582,13 +655,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF00B050"/>
       </font>
@@ -606,13 +672,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF00B050"/>
       </font>
@@ -630,13 +689,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF00B050"/>
       </font>
@@ -654,13 +706,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF00B050"/>
       </font>
@@ -678,13 +723,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF00B050"/>
       </font>
@@ -702,13 +740,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF00B050"/>
       </font>
@@ -726,13 +757,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF00B050"/>
       </font>
@@ -750,13 +774,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF00B050"/>
       </font>
@@ -774,13 +791,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF00B050"/>
       </font>
@@ -798,13 +808,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF00B050"/>
       </font>
@@ -1041,210 +1044,6 @@
           <bgColor rgb="FFFFE699"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
     </dxf>
     <dxf>
       <fill>
@@ -1729,7 +1528,7 @@
         <v>25</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>26</v>
@@ -1739,10 +1538,11 @@
       <c r="A15" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6" t="str">
+        <f>IF(ISBLANK(B15),"Not Done",B15)</f>
+        <v>Not Done</v>
+      </c>
       <c r="J15" t="s">
         <v>27</v>
       </c>
@@ -1757,7 +1557,7 @@
         <v>25</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>26</v>
@@ -1767,10 +1567,11 @@
       <c r="A19" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6" t="str">
+        <f>IF(ISBLANK(B19),"Not Done",B19)</f>
+        <v>Not Done</v>
+      </c>
       <c r="J19" t="s">
         <v>27</v>
       </c>
@@ -2916,7 +2717,7 @@
         <v>25</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>26</v>
@@ -2926,12 +2727,10 @@
       <c r="A74" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B74" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C74" s="6"/>
-      <c r="J74" t="s">
-        <v>27</v>
+      <c r="B74" s="6"/>
+      <c r="C74" s="6" t="str">
+        <f>IF(ISBLANK(B74),"Not Done",B74)</f>
+        <v>Not Done</v>
       </c>
       <c r="N74" s="10" t="s">
         <v>80</v>
@@ -2956,12 +2755,10 @@
       <c r="A75" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B75" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C75" s="6"/>
-      <c r="J75" t="s">
-        <v>27</v>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6" t="str">
+        <f t="shared" ref="C75:C77" si="0">IF(ISBLANK(B75),"Not Done",B75)</f>
+        <v>Not Done</v>
       </c>
       <c r="N75" s="10" t="s">
         <v>80</v>
@@ -2986,12 +2783,10 @@
       <c r="A76" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B76" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C76" s="6"/>
-      <c r="J76" t="s">
-        <v>27</v>
+      <c r="B76" s="6"/>
+      <c r="C76" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Done</v>
       </c>
       <c r="N76" s="10" t="s">
         <v>80</v>
@@ -3016,12 +2811,10 @@
       <c r="A77" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B77" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C77" s="6"/>
-      <c r="J77" t="s">
-        <v>27</v>
+      <c r="B77" s="6"/>
+      <c r="C77" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Done</v>
       </c>
       <c r="N77" s="10" t="s">
         <v>80</v>
@@ -3052,7 +2845,7 @@
         <v>25</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>26</v>
@@ -3062,12 +2855,10 @@
       <c r="A81" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B81" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C81" s="6"/>
-      <c r="J81" t="s">
-        <v>27</v>
+      <c r="B81" s="6"/>
+      <c r="C81" s="6" t="str">
+        <f>IF(ISBLANK(B81),"Not Done",B81)</f>
+        <v>Not Done</v>
       </c>
       <c r="N81" s="10" t="s">
         <v>80</v>
@@ -3092,12 +2883,10 @@
       <c r="A82" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B82" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C82" s="6"/>
-      <c r="J82" t="s">
-        <v>27</v>
+      <c r="B82" s="6"/>
+      <c r="C82" s="6" t="str">
+        <f t="shared" ref="C82:C84" si="1">IF(ISBLANK(B82),"Not Done",B82)</f>
+        <v>Not Done</v>
       </c>
       <c r="N82" s="10" t="s">
         <v>80</v>
@@ -3122,12 +2911,10 @@
       <c r="A83" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B83" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C83" s="6"/>
-      <c r="J83" t="s">
-        <v>27</v>
+      <c r="B83" s="6"/>
+      <c r="C83" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Not Done</v>
       </c>
       <c r="N83" s="10" t="s">
         <v>80</v>
@@ -3152,12 +2939,10 @@
       <c r="A84" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B84" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C84" s="6"/>
-      <c r="J84" t="s">
-        <v>27</v>
+      <c r="B84" s="6"/>
+      <c r="C84" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Not Done</v>
       </c>
       <c r="N84" s="10" t="s">
         <v>80</v>
@@ -3188,7 +2973,7 @@
         <v>25</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="C87" s="5" t="s">
         <v>26</v>
@@ -3198,12 +2983,10 @@
       <c r="A88" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B88" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C88" s="6"/>
-      <c r="J88" t="s">
-        <v>27</v>
+      <c r="B88" s="6"/>
+      <c r="C88" s="6" t="str">
+        <f>IF(ISBLANK(B88),"Not Done",B88)</f>
+        <v>Not Done</v>
       </c>
       <c r="N88" s="10" t="s">
         <v>80</v>
@@ -3228,12 +3011,10 @@
       <c r="A89" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B89" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C89" s="6"/>
-      <c r="J89" t="s">
-        <v>27</v>
+      <c r="B89" s="6"/>
+      <c r="C89" s="6" t="str">
+        <f t="shared" ref="C89:C91" si="2">IF(ISBLANK(B89),"Not Done",B89)</f>
+        <v>Not Done</v>
       </c>
       <c r="N89" s="10" t="s">
         <v>80</v>
@@ -3258,12 +3039,10 @@
       <c r="A90" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B90" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C90" s="6"/>
-      <c r="J90" t="s">
-        <v>27</v>
+      <c r="B90" s="6"/>
+      <c r="C90" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>Not Done</v>
       </c>
       <c r="N90" s="10" t="s">
         <v>80</v>
@@ -3288,12 +3067,10 @@
       <c r="A91" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B91" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C91" s="6"/>
-      <c r="J91" t="s">
-        <v>27</v>
+      <c r="B91" s="6"/>
+      <c r="C91" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>Not Done</v>
       </c>
       <c r="N91" s="10" t="s">
         <v>80</v>
@@ -3324,7 +3101,7 @@
         <v>25</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="C94" s="5" t="s">
         <v>26</v>
@@ -3334,12 +3111,10 @@
       <c r="A95" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B95" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C95" s="6"/>
-      <c r="J95" t="s">
-        <v>27</v>
+      <c r="B95" s="6"/>
+      <c r="C95" s="6" t="str">
+        <f>IF(ISBLANK(B95),"Not Done",B95)</f>
+        <v>Not Done</v>
       </c>
       <c r="N95" s="10" t="s">
         <v>80</v>
@@ -3364,12 +3139,10 @@
       <c r="A96" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B96" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C96" s="6"/>
-      <c r="J96" t="s">
-        <v>27</v>
+      <c r="B96" s="6"/>
+      <c r="C96" s="6" t="str">
+        <f t="shared" ref="C96:C98" si="3">IF(ISBLANK(B96),"Not Done",B96)</f>
+        <v>Not Done</v>
       </c>
       <c r="N96" s="10" t="s">
         <v>80</v>
@@ -3394,12 +3167,10 @@
       <c r="A97" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B97" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C97" s="6"/>
-      <c r="J97" t="s">
-        <v>27</v>
+      <c r="B97" s="6"/>
+      <c r="C97" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Not Done</v>
       </c>
       <c r="N97" s="10" t="s">
         <v>80</v>
@@ -3424,12 +3195,10 @@
       <c r="A98" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B98" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C98" s="6"/>
-      <c r="J98" t="s">
-        <v>27</v>
+      <c r="B98" s="6"/>
+      <c r="C98" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Not Done</v>
       </c>
       <c r="N98" s="10" t="s">
         <v>80</v>
@@ -3510,646 +3279,514 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B5">
-    <cfRule type="containsText" dxfId="152" priority="1" operator="containsText" text="highlight">
+    <cfRule type="containsText" dxfId="116" priority="16" operator="containsText" text="highlight">
       <formula>ISBLANK(B5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="containsText" dxfId="151" priority="2" operator="containsText" text="highlight">
+    <cfRule type="containsText" dxfId="115" priority="17" operator="containsText" text="highlight">
       <formula>ISBLANK(F5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="containsText" dxfId="150" priority="3" operator="containsText" text="highlight">
+    <cfRule type="containsText" dxfId="114" priority="18" operator="containsText" text="highlight">
       <formula>ISBLANK(B7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="containsText" dxfId="149" priority="4" operator="containsText" text="highlight">
+    <cfRule type="containsText" dxfId="113" priority="19" operator="containsText" text="highlight">
       <formula>ISBLANK(F9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="containsText" dxfId="148" priority="5" operator="containsText" text="highlight">
+    <cfRule type="containsText" dxfId="112" priority="20" operator="containsText" text="highlight">
       <formula>ISBLANK(B11)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="containsText" dxfId="147" priority="6" operator="containsText" text="highlight">
+    <cfRule type="containsText" dxfId="111" priority="21" operator="containsText" text="highlight">
       <formula>ISBLANK(F10)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="containsText" dxfId="146" priority="7" operator="containsText" text="highlight">
+    <cfRule type="containsText" dxfId="110" priority="22" operator="containsText" text="highlight">
       <formula>ISBLANK(B15)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B19">
+    <cfRule type="containsText" dxfId="109" priority="26" operator="containsText" text="highlight">
+      <formula>ISBLANK(B19)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23">
+    <cfRule type="containsText" dxfId="108" priority="30" operator="containsText" text="highlight">
+      <formula>ISBLANK(D23)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G23">
+    <cfRule type="containsText" dxfId="107" priority="31" operator="containsText" text="highlight">
+      <formula>G23="Fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="106" priority="32" operator="containsText" text="highlight">
+      <formula>G23="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D24">
+    <cfRule type="containsText" dxfId="105" priority="33" operator="containsText" text="highlight">
+      <formula>ISBLANK(D24)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G24">
+    <cfRule type="containsText" dxfId="104" priority="34" operator="containsText" text="highlight">
+      <formula>G24="Fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="103" priority="35" operator="containsText" text="highlight">
+      <formula>G24="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D28">
+    <cfRule type="containsText" dxfId="102" priority="36" operator="containsText" text="highlight">
+      <formula>ISBLANK(D28)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G28">
+    <cfRule type="containsText" dxfId="101" priority="37" operator="containsText" text="highlight">
+      <formula>G28="Fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="100" priority="38" operator="containsText" text="highlight">
+      <formula>G28="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D29">
+    <cfRule type="containsText" dxfId="99" priority="39" operator="containsText" text="highlight">
+      <formula>ISBLANK(D29)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G29">
+    <cfRule type="containsText" dxfId="98" priority="40" operator="containsText" text="highlight">
+      <formula>G29="Fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="97" priority="41" operator="containsText" text="highlight">
+      <formula>G29="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33">
+    <cfRule type="containsText" dxfId="96" priority="42" operator="containsText" text="highlight">
+      <formula>ISBLANK(D33)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G33">
+    <cfRule type="containsText" dxfId="95" priority="43" operator="containsText" text="highlight">
+      <formula>G33="Fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="94" priority="44" operator="containsText" text="highlight">
+      <formula>G33="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34">
+    <cfRule type="containsText" dxfId="93" priority="45" operator="containsText" text="highlight">
+      <formula>ISBLANK(D34)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G34">
+    <cfRule type="containsText" dxfId="92" priority="46" operator="containsText" text="highlight">
+      <formula>G34="Fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="91" priority="47" operator="containsText" text="highlight">
+      <formula>G34="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38">
+    <cfRule type="containsText" dxfId="90" priority="48" operator="containsText" text="highlight">
+      <formula>ISBLANK(D38)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G38">
+    <cfRule type="containsText" dxfId="89" priority="49" operator="containsText" text="highlight">
+      <formula>G38="Fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="88" priority="50" operator="containsText" text="highlight">
+      <formula>G38="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D39">
+    <cfRule type="containsText" dxfId="87" priority="51" operator="containsText" text="highlight">
+      <formula>ISBLANK(D39)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G39">
+    <cfRule type="containsText" dxfId="86" priority="52" operator="containsText" text="highlight">
+      <formula>G39="Fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="85" priority="53" operator="containsText" text="highlight">
+      <formula>G39="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D43">
+    <cfRule type="containsText" dxfId="84" priority="54" operator="containsText" text="highlight">
+      <formula>ISBLANK(D43)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G43">
+    <cfRule type="containsText" dxfId="83" priority="55" operator="containsText" text="highlight">
+      <formula>G43="Fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="82" priority="56" operator="containsText" text="highlight">
+      <formula>G43="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D44">
+    <cfRule type="containsText" dxfId="81" priority="57" operator="containsText" text="highlight">
+      <formula>ISBLANK(D44)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G44">
+    <cfRule type="containsText" dxfId="80" priority="58" operator="containsText" text="highlight">
+      <formula>G44="Fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="79" priority="59" operator="containsText" text="highlight">
+      <formula>G44="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D45">
+    <cfRule type="containsText" dxfId="78" priority="60" operator="containsText" text="highlight">
+      <formula>ISBLANK(D45)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G45">
+    <cfRule type="containsText" dxfId="77" priority="61" operator="containsText" text="highlight">
+      <formula>G45="Fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="76" priority="62" operator="containsText" text="highlight">
+      <formula>G45="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D49">
+    <cfRule type="containsText" dxfId="75" priority="63" operator="containsText" text="highlight">
+      <formula>ISBLANK(D49)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G49">
+    <cfRule type="containsText" dxfId="74" priority="64" operator="containsText" text="highlight">
+      <formula>G49="Fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="73" priority="65" operator="containsText" text="highlight">
+      <formula>G49="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D50">
+    <cfRule type="containsText" dxfId="72" priority="66" operator="containsText" text="highlight">
+      <formula>ISBLANK(D50)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G50">
+    <cfRule type="containsText" dxfId="71" priority="67" operator="containsText" text="highlight">
+      <formula>G50="Fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="70" priority="68" operator="containsText" text="highlight">
+      <formula>G50="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D51">
+    <cfRule type="containsText" dxfId="69" priority="69" operator="containsText" text="highlight">
+      <formula>ISBLANK(D51)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G51">
+    <cfRule type="containsText" dxfId="68" priority="70" operator="containsText" text="highlight">
+      <formula>G51="Fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="67" priority="71" operator="containsText" text="highlight">
+      <formula>G51="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D55">
+    <cfRule type="containsText" dxfId="66" priority="72" operator="containsText" text="highlight">
+      <formula>ISBLANK(D55)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G55">
+    <cfRule type="containsText" dxfId="65" priority="73" operator="containsText" text="highlight">
+      <formula>G55="Fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="64" priority="74" operator="containsText" text="highlight">
+      <formula>G55="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D56">
+    <cfRule type="containsText" dxfId="63" priority="75" operator="containsText" text="highlight">
+      <formula>ISBLANK(D56)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G56">
+    <cfRule type="containsText" dxfId="62" priority="76" operator="containsText" text="highlight">
+      <formula>G56="Fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="61" priority="77" operator="containsText" text="highlight">
+      <formula>G56="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D57">
+    <cfRule type="containsText" dxfId="60" priority="78" operator="containsText" text="highlight">
+      <formula>ISBLANK(D57)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G57">
+    <cfRule type="containsText" dxfId="59" priority="79" operator="containsText" text="highlight">
+      <formula>G57="Fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="58" priority="80" operator="containsText" text="highlight">
+      <formula>G57="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D61">
+    <cfRule type="containsText" dxfId="57" priority="81" operator="containsText" text="highlight">
+      <formula>ISBLANK(D61)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G61">
+    <cfRule type="containsText" dxfId="56" priority="82" operator="containsText" text="highlight">
+      <formula>G61="Fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="55" priority="83" operator="containsText" text="highlight">
+      <formula>G61="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D62">
+    <cfRule type="containsText" dxfId="54" priority="84" operator="containsText" text="highlight">
+      <formula>ISBLANK(D62)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G62">
+    <cfRule type="containsText" dxfId="53" priority="85" operator="containsText" text="highlight">
+      <formula>G62="Fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="52" priority="86" operator="containsText" text="highlight">
+      <formula>G62="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D63">
+    <cfRule type="containsText" dxfId="51" priority="87" operator="containsText" text="highlight">
+      <formula>ISBLANK(D63)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G63">
+    <cfRule type="containsText" dxfId="50" priority="88" operator="containsText" text="highlight">
+      <formula>G63="Fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="49" priority="89" operator="containsText" text="highlight">
+      <formula>G63="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B67">
+    <cfRule type="containsText" dxfId="48" priority="90" operator="containsText" text="highlight">
+      <formula>ISBLANK(B67)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F67">
+    <cfRule type="containsText" dxfId="47" priority="91" operator="containsText" text="highlight">
+      <formula>F67="Fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="46" priority="92" operator="containsText" text="highlight">
+      <formula>F67="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B68">
+    <cfRule type="containsText" dxfId="45" priority="93" operator="containsText" text="highlight">
+      <formula>ISBLANK(B68)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F68">
+    <cfRule type="containsText" dxfId="44" priority="94" operator="containsText" text="highlight">
+      <formula>F68="Fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="43" priority="95" operator="containsText" text="highlight">
+      <formula>F68="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B69">
+    <cfRule type="containsText" dxfId="42" priority="96" operator="containsText" text="highlight">
+      <formula>ISBLANK(B69)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F69">
+    <cfRule type="containsText" dxfId="41" priority="97" operator="containsText" text="highlight">
+      <formula>F69="Fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="98" operator="containsText" text="highlight">
+      <formula>F69="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B70">
+    <cfRule type="containsText" dxfId="39" priority="99" operator="containsText" text="highlight">
+      <formula>ISBLANK(B70)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F70">
+    <cfRule type="containsText" dxfId="38" priority="100" operator="containsText" text="highlight">
+      <formula>F70="Fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="101" operator="containsText" text="highlight">
+      <formula>F70="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B74">
+    <cfRule type="containsText" dxfId="36" priority="102" operator="containsText" text="highlight">
+      <formula>ISBLANK(B74)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C74:C77">
+    <cfRule type="containsText" dxfId="35" priority="103" operator="containsText" text="highlight">
+      <formula>ISBLANK(C74)</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="104" operator="containsText" text="highlight">
+      <formula>C74="Fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="33" priority="105" operator="containsText" text="highlight">
+      <formula>C74="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B75">
+    <cfRule type="containsText" dxfId="32" priority="106" operator="containsText" text="highlight">
+      <formula>ISBLANK(B75)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B76">
+    <cfRule type="containsText" dxfId="31" priority="110" operator="containsText" text="highlight">
+      <formula>ISBLANK(B76)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B77">
+    <cfRule type="containsText" dxfId="30" priority="114" operator="containsText" text="highlight">
+      <formula>ISBLANK(B77)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B81">
+    <cfRule type="containsText" dxfId="29" priority="118" operator="containsText" text="highlight">
+      <formula>ISBLANK(B81)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B82">
+    <cfRule type="containsText" dxfId="28" priority="122" operator="containsText" text="highlight">
+      <formula>ISBLANK(B82)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83">
+    <cfRule type="containsText" dxfId="27" priority="126" operator="containsText" text="highlight">
+      <formula>ISBLANK(B83)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B84">
+    <cfRule type="containsText" dxfId="26" priority="130" operator="containsText" text="highlight">
+      <formula>ISBLANK(B84)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B88">
+    <cfRule type="containsText" dxfId="25" priority="134" operator="containsText" text="highlight">
+      <formula>ISBLANK(B88)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B89">
+    <cfRule type="containsText" dxfId="24" priority="138" operator="containsText" text="highlight">
+      <formula>ISBLANK(B89)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B90">
+    <cfRule type="containsText" dxfId="23" priority="142" operator="containsText" text="highlight">
+      <formula>ISBLANK(B90)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B91">
+    <cfRule type="containsText" dxfId="22" priority="146" operator="containsText" text="highlight">
+      <formula>ISBLANK(B91)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B95">
+    <cfRule type="containsText" dxfId="21" priority="150" operator="containsText" text="highlight">
+      <formula>ISBLANK(B95)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B96">
+    <cfRule type="containsText" dxfId="20" priority="154" operator="containsText" text="highlight">
+      <formula>ISBLANK(B96)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B97">
+    <cfRule type="containsText" dxfId="19" priority="158" operator="containsText" text="highlight">
+      <formula>ISBLANK(B97)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B98">
+    <cfRule type="containsText" dxfId="18" priority="162" operator="containsText" text="highlight">
+      <formula>ISBLANK(B98)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C102">
+    <cfRule type="containsText" dxfId="17" priority="166" operator="containsText" text="highlight">
+      <formula>ISBLANK(C102)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F102">
+    <cfRule type="containsText" dxfId="16" priority="167" operator="containsText" text="highlight">
+      <formula>F102="Fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="168" operator="containsText" text="highlight">
+      <formula>F102="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C81:C84">
+    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="highlight">
+      <formula>ISBLANK(C81)</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="highlight">
+      <formula>C81="Fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="highlight">
+      <formula>C81="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C88:C91">
+    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="highlight">
+      <formula>ISBLANK(C88)</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="highlight">
+      <formula>C88="Fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="highlight">
+      <formula>C88="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C95:C98">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="highlight">
+      <formula>ISBLANK(C95)</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="highlight">
+      <formula>C95="Fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="highlight">
+      <formula>C95="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="containsText" dxfId="145" priority="8" operator="containsText" text="highlight">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="highlight">
       <formula>ISBLANK(C15)</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="144" priority="9" operator="containsText" text="highlight">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="highlight">
       <formula>C15="Fail"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="143" priority="10" operator="containsText" text="highlight">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="highlight">
       <formula>C15="Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19">
-    <cfRule type="containsText" dxfId="142" priority="11" operator="containsText" text="highlight">
-      <formula>ISBLANK(B19)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="141" priority="12" operator="containsText" text="highlight">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="highlight">
       <formula>ISBLANK(C19)</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="140" priority="13" operator="containsText" text="highlight">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="highlight">
       <formula>C19="Fail"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="139" priority="14" operator="containsText" text="highlight">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="highlight">
       <formula>C19="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D23">
-    <cfRule type="containsText" dxfId="138" priority="15" operator="containsText" text="highlight">
-      <formula>ISBLANK(D23)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G23">
-    <cfRule type="containsText" dxfId="137" priority="16" operator="containsText" text="highlight">
-      <formula>G23="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="136" priority="17" operator="containsText" text="highlight">
-      <formula>G23="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D24">
-    <cfRule type="containsText" dxfId="135" priority="18" operator="containsText" text="highlight">
-      <formula>ISBLANK(D24)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G24">
-    <cfRule type="containsText" dxfId="134" priority="19" operator="containsText" text="highlight">
-      <formula>G24="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="133" priority="20" operator="containsText" text="highlight">
-      <formula>G24="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D28">
-    <cfRule type="containsText" dxfId="132" priority="21" operator="containsText" text="highlight">
-      <formula>ISBLANK(D28)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G28">
-    <cfRule type="containsText" dxfId="131" priority="22" operator="containsText" text="highlight">
-      <formula>G28="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="23" operator="containsText" text="highlight">
-      <formula>G28="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D29">
-    <cfRule type="containsText" dxfId="129" priority="24" operator="containsText" text="highlight">
-      <formula>ISBLANK(D29)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G29">
-    <cfRule type="containsText" dxfId="128" priority="25" operator="containsText" text="highlight">
-      <formula>G29="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="127" priority="26" operator="containsText" text="highlight">
-      <formula>G29="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D33">
-    <cfRule type="containsText" dxfId="126" priority="27" operator="containsText" text="highlight">
-      <formula>ISBLANK(D33)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G33">
-    <cfRule type="containsText" dxfId="125" priority="28" operator="containsText" text="highlight">
-      <formula>G33="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="124" priority="29" operator="containsText" text="highlight">
-      <formula>G33="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
-    <cfRule type="containsText" dxfId="123" priority="30" operator="containsText" text="highlight">
-      <formula>ISBLANK(D34)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G34">
-    <cfRule type="containsText" dxfId="122" priority="31" operator="containsText" text="highlight">
-      <formula>G34="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="32" operator="containsText" text="highlight">
-      <formula>G34="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D38">
-    <cfRule type="containsText" dxfId="120" priority="33" operator="containsText" text="highlight">
-      <formula>ISBLANK(D38)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G38">
-    <cfRule type="containsText" dxfId="119" priority="34" operator="containsText" text="highlight">
-      <formula>G38="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="35" operator="containsText" text="highlight">
-      <formula>G38="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D39">
-    <cfRule type="containsText" dxfId="117" priority="36" operator="containsText" text="highlight">
-      <formula>ISBLANK(D39)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G39">
-    <cfRule type="containsText" dxfId="116" priority="37" operator="containsText" text="highlight">
-      <formula>G39="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="38" operator="containsText" text="highlight">
-      <formula>G39="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D43">
-    <cfRule type="containsText" dxfId="114" priority="39" operator="containsText" text="highlight">
-      <formula>ISBLANK(D43)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G43">
-    <cfRule type="containsText" dxfId="113" priority="40" operator="containsText" text="highlight">
-      <formula>G43="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="41" operator="containsText" text="highlight">
-      <formula>G43="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D44">
-    <cfRule type="containsText" dxfId="111" priority="42" operator="containsText" text="highlight">
-      <formula>ISBLANK(D44)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G44">
-    <cfRule type="containsText" dxfId="110" priority="43" operator="containsText" text="highlight">
-      <formula>G44="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="44" operator="containsText" text="highlight">
-      <formula>G44="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D45">
-    <cfRule type="containsText" dxfId="108" priority="45" operator="containsText" text="highlight">
-      <formula>ISBLANK(D45)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G45">
-    <cfRule type="containsText" dxfId="107" priority="46" operator="containsText" text="highlight">
-      <formula>G45="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="47" operator="containsText" text="highlight">
-      <formula>G45="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D49">
-    <cfRule type="containsText" dxfId="105" priority="48" operator="containsText" text="highlight">
-      <formula>ISBLANK(D49)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G49">
-    <cfRule type="containsText" dxfId="104" priority="49" operator="containsText" text="highlight">
-      <formula>G49="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="50" operator="containsText" text="highlight">
-      <formula>G49="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D50">
-    <cfRule type="containsText" dxfId="102" priority="51" operator="containsText" text="highlight">
-      <formula>ISBLANK(D50)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G50">
-    <cfRule type="containsText" dxfId="101" priority="52" operator="containsText" text="highlight">
-      <formula>G50="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="53" operator="containsText" text="highlight">
-      <formula>G50="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D51">
-    <cfRule type="containsText" dxfId="99" priority="54" operator="containsText" text="highlight">
-      <formula>ISBLANK(D51)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G51">
-    <cfRule type="containsText" dxfId="98" priority="55" operator="containsText" text="highlight">
-      <formula>G51="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="56" operator="containsText" text="highlight">
-      <formula>G51="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D55">
-    <cfRule type="containsText" dxfId="96" priority="57" operator="containsText" text="highlight">
-      <formula>ISBLANK(D55)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G55">
-    <cfRule type="containsText" dxfId="95" priority="58" operator="containsText" text="highlight">
-      <formula>G55="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="59" operator="containsText" text="highlight">
-      <formula>G55="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D56">
-    <cfRule type="containsText" dxfId="93" priority="60" operator="containsText" text="highlight">
-      <formula>ISBLANK(D56)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G56">
-    <cfRule type="containsText" dxfId="92" priority="61" operator="containsText" text="highlight">
-      <formula>G56="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="62" operator="containsText" text="highlight">
-      <formula>G56="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D57">
-    <cfRule type="containsText" dxfId="90" priority="63" operator="containsText" text="highlight">
-      <formula>ISBLANK(D57)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G57">
-    <cfRule type="containsText" dxfId="89" priority="64" operator="containsText" text="highlight">
-      <formula>G57="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="65" operator="containsText" text="highlight">
-      <formula>G57="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D61">
-    <cfRule type="containsText" dxfId="87" priority="66" operator="containsText" text="highlight">
-      <formula>ISBLANK(D61)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G61">
-    <cfRule type="containsText" dxfId="86" priority="67" operator="containsText" text="highlight">
-      <formula>G61="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="68" operator="containsText" text="highlight">
-      <formula>G61="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D62">
-    <cfRule type="containsText" dxfId="84" priority="69" operator="containsText" text="highlight">
-      <formula>ISBLANK(D62)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G62">
-    <cfRule type="containsText" dxfId="83" priority="70" operator="containsText" text="highlight">
-      <formula>G62="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="71" operator="containsText" text="highlight">
-      <formula>G62="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D63">
-    <cfRule type="containsText" dxfId="81" priority="72" operator="containsText" text="highlight">
-      <formula>ISBLANK(D63)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G63">
-    <cfRule type="containsText" dxfId="80" priority="73" operator="containsText" text="highlight">
-      <formula>G63="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="74" operator="containsText" text="highlight">
-      <formula>G63="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B67">
-    <cfRule type="containsText" dxfId="78" priority="75" operator="containsText" text="highlight">
-      <formula>ISBLANK(B67)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F67">
-    <cfRule type="containsText" dxfId="77" priority="76" operator="containsText" text="highlight">
-      <formula>F67="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="77" operator="containsText" text="highlight">
-      <formula>F67="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B68">
-    <cfRule type="containsText" dxfId="75" priority="78" operator="containsText" text="highlight">
-      <formula>ISBLANK(B68)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F68">
-    <cfRule type="containsText" dxfId="74" priority="79" operator="containsText" text="highlight">
-      <formula>F68="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="80" operator="containsText" text="highlight">
-      <formula>F68="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B69">
-    <cfRule type="containsText" dxfId="72" priority="81" operator="containsText" text="highlight">
-      <formula>ISBLANK(B69)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F69">
-    <cfRule type="containsText" dxfId="71" priority="82" operator="containsText" text="highlight">
-      <formula>F69="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="83" operator="containsText" text="highlight">
-      <formula>F69="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B70">
-    <cfRule type="containsText" dxfId="69" priority="84" operator="containsText" text="highlight">
-      <formula>ISBLANK(B70)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F70">
-    <cfRule type="containsText" dxfId="68" priority="85" operator="containsText" text="highlight">
-      <formula>F70="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="86" operator="containsText" text="highlight">
-      <formula>F70="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B74">
-    <cfRule type="containsText" dxfId="66" priority="87" operator="containsText" text="highlight">
-      <formula>ISBLANK(B74)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C74">
-    <cfRule type="containsText" dxfId="65" priority="88" operator="containsText" text="highlight">
-      <formula>ISBLANK(C74)</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="89" operator="containsText" text="highlight">
-      <formula>C74="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="90" operator="containsText" text="highlight">
-      <formula>C74="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B75">
-    <cfRule type="containsText" dxfId="62" priority="91" operator="containsText" text="highlight">
-      <formula>ISBLANK(B75)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C75">
-    <cfRule type="containsText" dxfId="61" priority="92" operator="containsText" text="highlight">
-      <formula>ISBLANK(C75)</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="93" operator="containsText" text="highlight">
-      <formula>C75="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="94" operator="containsText" text="highlight">
-      <formula>C75="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B76">
-    <cfRule type="containsText" dxfId="58" priority="95" operator="containsText" text="highlight">
-      <formula>ISBLANK(B76)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C76">
-    <cfRule type="containsText" dxfId="57" priority="96" operator="containsText" text="highlight">
-      <formula>ISBLANK(C76)</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="97" operator="containsText" text="highlight">
-      <formula>C76="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="98" operator="containsText" text="highlight">
-      <formula>C76="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B77">
-    <cfRule type="containsText" dxfId="54" priority="99" operator="containsText" text="highlight">
-      <formula>ISBLANK(B77)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C77">
-    <cfRule type="containsText" dxfId="53" priority="100" operator="containsText" text="highlight">
-      <formula>ISBLANK(C77)</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="101" operator="containsText" text="highlight">
-      <formula>C77="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="102" operator="containsText" text="highlight">
-      <formula>C77="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B81">
-    <cfRule type="containsText" dxfId="50" priority="103" operator="containsText" text="highlight">
-      <formula>ISBLANK(B81)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C81">
-    <cfRule type="containsText" dxfId="49" priority="104" operator="containsText" text="highlight">
-      <formula>ISBLANK(C81)</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="105" operator="containsText" text="highlight">
-      <formula>C81="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="106" operator="containsText" text="highlight">
-      <formula>C81="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B82">
-    <cfRule type="containsText" dxfId="46" priority="107" operator="containsText" text="highlight">
-      <formula>ISBLANK(B82)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C82">
-    <cfRule type="containsText" dxfId="45" priority="108" operator="containsText" text="highlight">
-      <formula>ISBLANK(C82)</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="109" operator="containsText" text="highlight">
-      <formula>C82="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="110" operator="containsText" text="highlight">
-      <formula>C82="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B83">
-    <cfRule type="containsText" dxfId="42" priority="111" operator="containsText" text="highlight">
-      <formula>ISBLANK(B83)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C83">
-    <cfRule type="containsText" dxfId="41" priority="112" operator="containsText" text="highlight">
-      <formula>ISBLANK(C83)</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="113" operator="containsText" text="highlight">
-      <formula>C83="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="114" operator="containsText" text="highlight">
-      <formula>C83="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B84">
-    <cfRule type="containsText" dxfId="38" priority="115" operator="containsText" text="highlight">
-      <formula>ISBLANK(B84)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C84">
-    <cfRule type="containsText" dxfId="37" priority="116" operator="containsText" text="highlight">
-      <formula>ISBLANK(C84)</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="117" operator="containsText" text="highlight">
-      <formula>C84="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="118" operator="containsText" text="highlight">
-      <formula>C84="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B88">
-    <cfRule type="containsText" dxfId="34" priority="119" operator="containsText" text="highlight">
-      <formula>ISBLANK(B88)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C88">
-    <cfRule type="containsText" dxfId="33" priority="120" operator="containsText" text="highlight">
-      <formula>ISBLANK(C88)</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="121" operator="containsText" text="highlight">
-      <formula>C88="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="122" operator="containsText" text="highlight">
-      <formula>C88="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B89">
-    <cfRule type="containsText" dxfId="30" priority="123" operator="containsText" text="highlight">
-      <formula>ISBLANK(B89)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C89">
-    <cfRule type="containsText" dxfId="29" priority="124" operator="containsText" text="highlight">
-      <formula>ISBLANK(C89)</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="125" operator="containsText" text="highlight">
-      <formula>C89="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="126" operator="containsText" text="highlight">
-      <formula>C89="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B90">
-    <cfRule type="containsText" dxfId="26" priority="127" operator="containsText" text="highlight">
-      <formula>ISBLANK(B90)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C90">
-    <cfRule type="containsText" dxfId="25" priority="128" operator="containsText" text="highlight">
-      <formula>ISBLANK(C90)</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="129" operator="containsText" text="highlight">
-      <formula>C90="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="130" operator="containsText" text="highlight">
-      <formula>C90="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B91">
-    <cfRule type="containsText" dxfId="22" priority="131" operator="containsText" text="highlight">
-      <formula>ISBLANK(B91)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C91">
-    <cfRule type="containsText" dxfId="21" priority="132" operator="containsText" text="highlight">
-      <formula>ISBLANK(C91)</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="133" operator="containsText" text="highlight">
-      <formula>C91="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="134" operator="containsText" text="highlight">
-      <formula>C91="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B95">
-    <cfRule type="containsText" dxfId="18" priority="135" operator="containsText" text="highlight">
-      <formula>ISBLANK(B95)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C95">
-    <cfRule type="containsText" dxfId="17" priority="136" operator="containsText" text="highlight">
-      <formula>ISBLANK(C95)</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="137" operator="containsText" text="highlight">
-      <formula>C95="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="138" operator="containsText" text="highlight">
-      <formula>C95="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B96">
-    <cfRule type="containsText" dxfId="14" priority="139" operator="containsText" text="highlight">
-      <formula>ISBLANK(B96)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C96">
-    <cfRule type="containsText" dxfId="13" priority="140" operator="containsText" text="highlight">
-      <formula>ISBLANK(C96)</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="141" operator="containsText" text="highlight">
-      <formula>C96="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="142" operator="containsText" text="highlight">
-      <formula>C96="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B97">
-    <cfRule type="containsText" dxfId="10" priority="143" operator="containsText" text="highlight">
-      <formula>ISBLANK(B97)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C97">
-    <cfRule type="containsText" dxfId="9" priority="144" operator="containsText" text="highlight">
-      <formula>ISBLANK(C97)</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="145" operator="containsText" text="highlight">
-      <formula>C97="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="146" operator="containsText" text="highlight">
-      <formula>C97="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B98">
-    <cfRule type="containsText" dxfId="6" priority="147" operator="containsText" text="highlight">
-      <formula>ISBLANK(B98)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C98">
-    <cfRule type="containsText" dxfId="5" priority="148" operator="containsText" text="highlight">
-      <formula>ISBLANK(C98)</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="149" operator="containsText" text="highlight">
-      <formula>C98="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="150" operator="containsText" text="highlight">
-      <formula>C98="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C102">
-    <cfRule type="containsText" dxfId="2" priority="151" operator="containsText" text="highlight">
-      <formula>ISBLANK(C102)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F102">
-    <cfRule type="containsText" dxfId="1" priority="152" operator="containsText" text="highlight">
-      <formula>F102="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="153" operator="containsText" text="highlight">
-      <formula>F102="Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updated for new columns
</commit_message>
<xml_diff>
--- a/testsheets/666_Tektronix_DPO20141.xlsx
+++ b/testsheets/666_Tektronix_DPO20141.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Software\Python\oscilloscope\testsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5ED815F5-DE25-43E3-B215-EEC77AF2A416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{29AE6A2C-3D62-49D6-96F6-52DE374BB251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="84">
   <si>
     <t>EMU Filename:</t>
   </si>
@@ -284,6 +284,12 @@
   </si>
   <si>
     <t>Result</t>
+  </si>
+  <si>
+    <t>Invert</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -306,23 +312,27 @@
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1402,10 +1412,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T104"/>
+  <dimension ref="A1:V104"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="B42" workbookViewId="0">
+      <selection activeCell="V64" sqref="V64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1547,12 +1557,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>25</v>
       </c>
@@ -1563,7 +1573,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>29</v>
       </c>
@@ -1576,7 +1586,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>30</v>
       </c>
@@ -1599,10 +1609,16 @@
         <v>74</v>
       </c>
       <c r="T21" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="U21" s="10" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V21" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>25</v>
       </c>
@@ -1623,7 +1639,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>35</v>
       </c>
@@ -1658,7 +1674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>37</v>
       </c>
@@ -1693,17 +1709,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D25" s="13"/>
     </row>
-    <row r="26" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B26" s="4"/>
       <c r="D26" s="13"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>25</v>
       </c>
@@ -1724,7 +1740,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>35</v>
       </c>
@@ -1759,7 +1775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>37</v>
       </c>
@@ -1794,17 +1810,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D30" s="13"/>
     </row>
-    <row r="31" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B31" s="4"/>
       <c r="D31" s="13"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>25</v>
       </c>
@@ -2164,7 +2180,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>42</v>
       </c>
@@ -2202,7 +2218,7 @@
         <v>1.7500000000000002E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>43</v>
       </c>
@@ -2240,7 +2256,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>45</v>
       </c>
@@ -2278,13 +2294,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B53" s="4"/>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>25</v>
       </c>
@@ -2305,7 +2321,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>42</v>
       </c>
@@ -2343,7 +2359,7 @@
         <v>1.7500000000000002E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>43</v>
       </c>
@@ -2381,7 +2397,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>45</v>
       </c>
@@ -2419,13 +2435,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B59" s="4"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>25</v>
       </c>
@@ -2446,7 +2462,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>42</v>
       </c>
@@ -2484,7 +2500,7 @@
         <v>1.7500000000000002E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
         <v>43</v>
       </c>
@@ -2521,8 +2537,11 @@
       <c r="S62" s="10">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V62" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
         <v>45</v>
       </c>
@@ -2558,6 +2577,9 @@
       </c>
       <c r="S63" s="10">
         <v>7</v>
+      </c>
+      <c r="V63" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>